<commit_message>
Update Gong PPT and Testing list etc.
</commit_message>
<xml_diff>
--- a/002Matlab Project/TesingList.xlsx
+++ b/002Matlab Project/TesingList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pgprogram\CM_Matting\002Matlab Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CM_Matting\002Matlab Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA0F10E-DC2E-48BD-8B5B-C374024E2A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F90D8C2-01A3-46E8-BD3B-9EEE09088336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9084" yWindow="108" windowWidth="13956" windowHeight="9972" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unittest" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="196">
   <si>
     <t>Use Case No.</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Pixels at BThreshold should be classified as foreground in frontImg.</t>
   </si>
   <si>
-    <t>Alpha Matte Calculation</t>
-  </si>
-  <si>
     <t>Test with uniform trimap</t>
   </si>
   <si>
@@ -427,12 +424,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Tse Case No.</t>
-  </si>
-  <si>
-    <t>Tse Case Description</t>
-  </si>
-  <si>
     <t>TC-001</t>
   </si>
   <si>
@@ -493,13 +484,7 @@
     <t>Foreground, background, and matte should be correctly generated despite the noise</t>
   </si>
   <si>
-    <t>Noise Handling</t>
-  </si>
-  <si>
     <t>Exception Handling</t>
-  </si>
-  <si>
-    <t>Performance Testing</t>
   </si>
   <si>
     <t>1. Execute the Bayesian_Matting function
@@ -609,13 +594,45 @@
   </si>
   <si>
     <t>UC-032</t>
+  </si>
+  <si>
+    <t>Alpha Matte Calculation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Background</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Preprocessing pics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case No.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Performance Testing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exception Handling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Noise Handling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -639,8 +656,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -650,6 +675,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -681,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -696,12 +727,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -709,6 +734,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -993,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:B33"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1012,58 +1056,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B2" s="10">
-        <v>1</v>
+        <v>156</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>190</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -1071,23 +1115,23 @@
     </row>
     <row r="3" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B3" s="10"/>
+        <v>157</v>
+      </c>
+      <c r="B3" s="8"/>
       <c r="C3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
@@ -1095,20 +1139,20 @@
     </row>
     <row r="4" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B4" s="10"/>
+        <v>158</v>
+      </c>
+      <c r="B4" s="8"/>
       <c r="C4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>11</v>
@@ -1119,20 +1163,20 @@
     </row>
     <row r="5" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B5" s="10"/>
+        <v>159</v>
+      </c>
+      <c r="B5" s="8"/>
       <c r="C5" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>12</v>
@@ -1143,23 +1187,23 @@
     </row>
     <row r="6" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B6" s="10"/>
+        <v>160</v>
+      </c>
+      <c r="B6" s="8"/>
       <c r="C6" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -1167,23 +1211,23 @@
     </row>
     <row r="7" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B7" s="10"/>
+        <v>161</v>
+      </c>
+      <c r="B7" s="8"/>
       <c r="C7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -1191,23 +1235,23 @@
     </row>
     <row r="8" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B8" s="10"/>
+        <v>162</v>
+      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -1215,23 +1259,23 @@
     </row>
     <row r="9" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B9" s="10"/>
+        <v>163</v>
+      </c>
+      <c r="B9" s="8"/>
       <c r="C9" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="G9" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -1239,25 +1283,25 @@
     </row>
     <row r="10" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B10" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="G10" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -1265,23 +1309,23 @@
     </row>
     <row r="11" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -1289,23 +1333,23 @@
     </row>
     <row r="12" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -1313,23 +1357,23 @@
     </row>
     <row r="13" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1337,23 +1381,23 @@
     </row>
     <row r="14" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="E14" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>52</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1361,23 +1405,23 @@
     </row>
     <row r="15" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -1385,23 +1429,23 @@
     </row>
     <row r="16" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -1409,23 +1453,23 @@
     </row>
     <row r="17" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="G17" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1433,25 +1477,25 @@
     </row>
     <row r="18" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B18" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1459,23 +1503,23 @@
     </row>
     <row r="19" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B19" s="10"/>
+        <v>173</v>
+      </c>
+      <c r="B19" s="8"/>
       <c r="C19" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -1483,23 +1527,23 @@
     </row>
     <row r="20" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B20" s="10"/>
+        <v>174</v>
+      </c>
+      <c r="B20" s="8"/>
       <c r="C20" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1507,23 +1551,23 @@
     </row>
     <row r="21" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B21" s="10"/>
+        <v>175</v>
+      </c>
+      <c r="B21" s="8"/>
       <c r="C21" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1531,23 +1575,23 @@
     </row>
     <row r="22" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B22" s="10"/>
+        <v>176</v>
+      </c>
+      <c r="B22" s="8"/>
       <c r="C22" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -1555,23 +1599,23 @@
     </row>
     <row r="23" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B23" s="10"/>
+        <v>177</v>
+      </c>
+      <c r="B23" s="8"/>
       <c r="C23" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -1579,23 +1623,23 @@
     </row>
     <row r="24" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B24" s="10"/>
+        <v>178</v>
+      </c>
+      <c r="B24" s="8"/>
       <c r="C24" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1603,23 +1647,23 @@
     </row>
     <row r="25" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B25" s="10"/>
+        <v>179</v>
+      </c>
+      <c r="B25" s="8"/>
       <c r="C25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -1627,25 +1671,25 @@
     </row>
     <row r="26" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B26" s="10">
-        <v>4</v>
-      </c>
-      <c r="C26" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="G26" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -1653,23 +1697,23 @@
     </row>
     <row r="27" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" s="10" t="s">
         <v>101</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -1677,23 +1721,23 @@
     </row>
     <row r="28" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D28" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="G28" s="10" t="s">
         <v>113</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -1701,23 +1745,23 @@
     </row>
     <row r="29" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="G29" s="10" t="s">
         <v>104</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -1725,23 +1769,23 @@
     </row>
     <row r="30" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>78</v>
+      <c r="G30" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -1749,23 +1793,23 @@
     </row>
     <row r="31" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="G31" s="10" t="s">
         <v>121</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -1773,23 +1817,23 @@
     </row>
     <row r="32" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="4" t="s">
+      <c r="F32" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="G32" s="10" t="s">
         <v>125</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -1797,23 +1841,23 @@
     </row>
     <row r="33" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D33" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="G33" s="10" t="s">
         <v>128</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -1836,164 +1880,162 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE3485A-70B3-44BC-B593-81EE8B29784F}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
+    <col min="4" max="6" width="34.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
     <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="E2" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="4" t="s">
+      <c r="B3" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="C3" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="E3" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="B4" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="C4" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="E4" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="1:9" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="B5" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="C5" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="E5" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="B6" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="F5" s="4" t="s">
+      <c r="C6" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="E6" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>